<commit_message>
Update report and status
</commit_message>
<xml_diff>
--- a/doc/Final Report Status.xlsx
+++ b/doc/Final Report Status.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10050"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="20670" windowHeight="10050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
   <si>
     <t>Section</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>Key Technical Elements</t>
-  </si>
-  <si>
-    <t>Performance Metrics Appendix</t>
   </si>
   <si>
     <t>Performance Metrics Summay</t>
@@ -172,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -181,6 +178,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,11 +480,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -499,63 +495,63 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>6</v>
+      <c r="A6" s="7" t="s">
+        <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -563,23 +559,23 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -587,7 +583,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -595,23 +591,23 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -619,54 +615,46 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="6" t="s">
+      <c r="B19" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="6" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="3" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish testing section and schematic/theory of operation/PCB section. Reformat to match CCup guideline of calibri 11 pt.
</commit_message>
<xml_diff>
--- a/doc/Final Report Status.xlsx
+++ b/doc/Final Report Status.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>Section</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Key Technical Elements</t>
   </si>
   <si>
-    <t>Performance Metrics Summay</t>
-  </si>
-  <si>
     <t>Failure Analysis</t>
   </si>
   <si>
@@ -95,14 +92,28 @@
   </si>
   <si>
     <t>Technical Documentation</t>
+  </si>
+  <si>
+    <t>Abstract</t>
+  </si>
+  <si>
+    <t>Performance Metrics</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -169,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -179,6 +190,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,7 +495,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -491,40 +506,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>18</v>
+      <c r="B1" s="10" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>2</v>
-      </c>
       <c r="B3" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>24</v>
@@ -532,7 +547,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>23</v>
@@ -540,121 +555,129 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="B10" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>10</v>
-      </c>
       <c r="B11" s="6" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>13</v>
+      <c r="A14" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>17</v>
-      </c>
       <c r="B17" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update report status, formatting fix
</commit_message>
<xml_diff>
--- a/doc/Final Report Status.xlsx
+++ b/doc/Final Report Status.xlsx
@@ -497,7 +497,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -554,7 +556,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="6" t="s">

</xml_diff>

<commit_message>
Include 2:24 battery life in report
</commit_message>
<xml_diff>
--- a/doc/Final Report Status.xlsx
+++ b/doc/Final Report Status.xlsx
@@ -49,9 +49,6 @@
     <t>Process Understanding</t>
   </si>
   <si>
-    <t>Reccomendations and next steps</t>
-  </si>
-  <si>
     <t>Glossary</t>
   </si>
   <si>
@@ -98,6 +95,9 @@
   </si>
   <si>
     <t>Performance Metrics</t>
+  </si>
+  <si>
+    <t>Recomendations and next steps</t>
   </si>
 </sst>
 </file>
@@ -180,20 +180,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,7 +497,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,178 +507,178 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>17</v>
+      <c r="B1" s="8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>24</v>
+      <c r="B4" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>24</v>
+      <c r="B5" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>23</v>
+      <c r="B6" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>22</v>
+      <c r="A7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>24</v>
+      <c r="B8" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>18</v>
+      <c r="B9" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>18</v>
+      <c r="B10" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>18</v>
+      <c r="B11" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="6" t="s">
+      <c r="B20" s="4" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>